<commit_message>
Update chi phí công ty, phân chia các dự án
</commit_message>
<xml_diff>
--- a/TongHopQuyCongTy.xlsx
+++ b/TongHopQuyCongTy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ViTechSolution_LTD\Team_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6173135-A0E0-466E-BAB4-B0C1746A7C38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64519FA8-E66D-4462-93BB-F888C63EDD07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thu" sheetId="2" r:id="rId1"/>
@@ -21,16 +21,18 @@
     <sheet name="Mua sắm linh kiện" sheetId="7" r:id="rId6"/>
     <sheet name="Chi phí thủ tục giấy tờ" sheetId="8" r:id="rId7"/>
     <sheet name="Chi phí nhân công" sheetId="9" r:id="rId8"/>
+    <sheet name="Cá nhân ứng tiền" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="Ca_nhan_ung_tien">'Cá nhân ứng tiền'!$O$3</definedName>
     <definedName name="Chi_phi_co_dinh">'Chi phí cố định'!$L$18</definedName>
     <definedName name="chi_phi_giay_to_thu_tuc">'Chi phí thủ tục giấy tờ'!$L$20</definedName>
     <definedName name="Chi_phi_hoat_dong">'Chi phí hoạt động'!$T$31</definedName>
     <definedName name="chi_phi_nhan_cong">'Chi phí nhân công'!$L$26</definedName>
-    <definedName name="mua_sam_linh_kien">'Mua sắm linh kiện'!$M$31</definedName>
+    <definedName name="mua_sam_linh_kien">'Mua sắm linh kiện'!$M$2</definedName>
     <definedName name="Mua_sam_thiet_bi">'Mua sắm thiết bị'!$O$19</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="120">
   <si>
     <t>Time</t>
   </si>
@@ -255,9 +257,6 @@
     <t>linh kien ngay 30.1</t>
   </si>
   <si>
-    <t>linh kieện ngày 20/02</t>
-  </si>
-  <si>
     <t>Mạch nạp stlink 7/03</t>
   </si>
   <si>
@@ -304,6 +303,105 @@
   </si>
   <si>
     <t>MS51</t>
+  </si>
+  <si>
+    <t>Cắt stencil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mua máy in </t>
+  </si>
+  <si>
+    <t>Mua Oscillator + IGBT</t>
+  </si>
+  <si>
+    <t>Thuê xe chuyển máy chạy + bàn</t>
+  </si>
+  <si>
+    <t>CK quyết toán thuế</t>
+  </si>
+  <si>
+    <t>CK thay đổi thông tin công ty</t>
+  </si>
+  <si>
+    <t>Tiền tk ACB</t>
+  </si>
+  <si>
+    <t>3 Con Xs3868</t>
+  </si>
+  <si>
+    <t>Ck mua linh kiện BT806 +BT966</t>
+  </si>
+  <si>
+    <t>Ck phi ship BT1006</t>
+  </si>
+  <si>
+    <t>Mua A2430</t>
+  </si>
+  <si>
+    <t>Đặt mạch in 22/02</t>
+  </si>
+  <si>
+    <t>Đặt mạch in 25/03</t>
+  </si>
+  <si>
+    <t>Mua linh kiện(Novuton 5)</t>
+  </si>
+  <si>
+    <t>Mua tụ, PL2303</t>
+  </si>
+  <si>
+    <t>Mua biến thế cách ly(Tuấn Oder)</t>
+  </si>
+  <si>
+    <t>Mua biến thế cách ly(Khơ Oder)</t>
+  </si>
+  <si>
+    <t>Đặt mạch in 30/03</t>
+  </si>
+  <si>
+    <t>Đặt mạch in 6/04</t>
+  </si>
+  <si>
+    <t>Mạch nạp + Mudule Nuvoton</t>
+  </si>
+  <si>
+    <t>Rashperry Pi 4 2G</t>
+  </si>
+  <si>
+    <t>Mua linh kiện Minh Hà</t>
+  </si>
+  <si>
+    <t>Tiền ăn trưa T7/CN (13-14/03)</t>
+  </si>
+  <si>
+    <t>Đặt cơm</t>
+  </si>
+  <si>
+    <t>13-14/03/21</t>
+  </si>
+  <si>
+    <t>Cá nhân ứng tiền</t>
+  </si>
+  <si>
+    <t>Ngày ứng</t>
+  </si>
+  <si>
+    <t>Số tiền</t>
+  </si>
+  <si>
+    <t>13/04/2021</t>
+  </si>
+  <si>
+    <t>linh kiện ngày 20/02</t>
+  </si>
+  <si>
+    <t>Thanh toán</t>
+  </si>
+  <si>
+    <t>Chưa thanh toán</t>
+  </si>
+  <si>
+    <t>Âm dự án trước</t>
   </si>
 </sst>
 </file>
@@ -313,7 +411,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$VND]\ #,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,8 +451,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0F5666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,18 +508,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -418,6 +527,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -469,7 +584,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -485,41 +599,101 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -530,8 +704,30 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -817,7 +1013,7 @@
   <dimension ref="H7:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,25 +1026,25 @@
   </cols>
   <sheetData>
     <row r="7" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H7" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
+      <c r="H7" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
     </row>
     <row r="9" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="37" t="s">
+      <c r="I9" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="28" t="s">
         <v>3</v>
       </c>
     </row>
@@ -884,11 +1080,11 @@
       <c r="J14" s="5"/>
     </row>
     <row r="20" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J20" s="35">
+      <c r="J20" s="26">
         <f>SUM(J10:J14)</f>
         <v>79000000</v>
       </c>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="25" t="s">
         <v>4</v>
       </c>
     </row>
@@ -903,107 +1099,165 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C944E29F-9B56-48EC-9427-F9273663C65B}">
-  <dimension ref="G4:N13"/>
+  <dimension ref="G4:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="48.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="1" customWidth="1"/>
     <col min="9" max="11" width="16.140625" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G4" s="39" t="s">
+    <row r="4" spans="7:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-    </row>
-    <row r="5" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-    </row>
-    <row r="6" spans="7:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="G6" s="27" t="s">
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="66">
+        <f>SUM(H7:H20)</f>
+        <v>87900480</v>
+      </c>
+      <c r="L4" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="63"/>
+    </row>
+    <row r="5" spans="7:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+    </row>
+    <row r="6" spans="7:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+    </row>
+    <row r="7" spans="7:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="G7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G7" s="32">
+      <c r="H7" s="5">
         <f>Chi_phi_co_dinh</f>
         <v>2500000</v>
       </c>
-      <c r="H7" s="32">
+      <c r="I7" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="7:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="G8" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="5">
         <f>Chi_phi_hoat_dong</f>
-        <v>2020000</v>
-      </c>
-      <c r="I7" s="32">
+        <v>2550000</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G9" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="5">
         <f>Mua_sam_thiet_bi</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="32">
+        <v>6950000</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G10" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="5">
         <f>mua_sam_linh_kien</f>
-        <v>20191480</v>
-      </c>
-      <c r="K7" s="32">
+        <v>28796480</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="7:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="G11" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="5">
         <f>chi_phi_giay_to_thu_tuc</f>
-        <v>2000000</v>
-      </c>
-      <c r="L7" s="32">
+        <v>6330000</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="7:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="G12" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="5">
         <f>chi_phi_nhan_cong</f>
         <v>3600000</v>
       </c>
-    </row>
-    <row r="13" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="M13" s="33">
-        <f>SUM(G7:L7)</f>
-        <v>30311480</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>4</v>
+      <c r="I12" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G13" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="5">
+        <f>Ca_nhan_ung_tien</f>
+        <v>37174000</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G4:L5"/>
+    <mergeCell ref="G4:I5"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:I13" xr:uid="{FB20CE85-9817-4FF7-81EF-BC82B065B869}">
+      <formula1>"Đã thanh toán, Chưa thanh toán"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G6" location="'Chi phí cố định'!A1" display="Chi phí cố định(Văn phòng làm việc, điện,nước)" xr:uid="{71F5C0D9-FAFD-4AFE-BBFE-E708C9915888}"/>
-    <hyperlink ref="H6" location="'Chi phí hoạt động'!A1" display="Chi phí hoạt động(ăn uống, trà nước, xe đi lại, liên hoan)" xr:uid="{9BEC1463-CA06-4FCB-91DF-132094BF6DC1}"/>
-    <hyperlink ref="I6" location="'Mua sắm thiết bị'!A1" display="Mua sắm thiết bị" xr:uid="{D0866C33-C75D-4E2A-AE85-197EDC2BB009}"/>
-    <hyperlink ref="J6" location="'Mua sắm linh kiện'!A1" display="Mua sắm linh kiện" xr:uid="{13E7C28D-5021-48C1-9397-447125DB223F}"/>
-    <hyperlink ref="K6" location="'Chi phí thủ tục giấy tờ'!A1" display="Chi phí thủ tục giấy tờ công ty" xr:uid="{A0D37EEE-050B-4A63-A122-6DA3C54B9868}"/>
-    <hyperlink ref="L6" location="'Chi phí nhân công'!A1" display="Chi phí nhân công + Hoa hồng môi giới dự án" xr:uid="{39F966DC-BB97-4D86-AC52-B077D0D01A2A}"/>
+    <hyperlink ref="G7" location="'Chi phí cố định'!A1" display="Chi phí cố định(Văn phòng làm việc, điện,nước)" xr:uid="{71F5C0D9-FAFD-4AFE-BBFE-E708C9915888}"/>
+    <hyperlink ref="G8" location="'Chi phí hoạt động'!A1" display="Chi phí hoạt động(ăn uống, trà nước, xe đi lại, liên hoan)" xr:uid="{9BEC1463-CA06-4FCB-91DF-132094BF6DC1}"/>
+    <hyperlink ref="G9" location="'Mua sắm thiết bị'!A1" display="Mua sắm thiết bị" xr:uid="{D0866C33-C75D-4E2A-AE85-197EDC2BB009}"/>
+    <hyperlink ref="G10" location="'Mua sắm linh kiện'!A1" display="Mua sắm linh kiện" xr:uid="{13E7C28D-5021-48C1-9397-447125DB223F}"/>
+    <hyperlink ref="G11" location="'Chi phí thủ tục giấy tờ'!A1" display="Chi phí thủ tục giấy tờ công ty" xr:uid="{A0D37EEE-050B-4A63-A122-6DA3C54B9868}"/>
+    <hyperlink ref="G12" location="'Chi phí nhân công'!A1" display="Chi phí nhân công + Hoa hồng môi giới dự án" xr:uid="{39F966DC-BB97-4D86-AC52-B077D0D01A2A}"/>
+    <hyperlink ref="G13" location="'Cá nhân ứng tiền'!A1" display="Cá nhân ứng tiền" xr:uid="{525798CB-DF6E-44C4-ABE0-80C344B09747}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1011,9 +1265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BD526D-A920-48D2-ABE4-92E53AD1E18B}">
   <dimension ref="A2:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1025,20 +1277,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="40"/>
+      <c r="K2" s="57"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="15" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1140,44 +1392,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F1DCA7F-675E-45DF-8131-5AD5A819A169}">
   <dimension ref="P3:U31"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="16" max="16" width="22.140625" customWidth="1"/>
     <col min="17" max="17" width="12.28515625" customWidth="1"/>
-    <col min="18" max="18" width="11" customWidth="1"/>
+    <col min="18" max="18" width="11" style="1" customWidth="1"/>
     <col min="20" max="20" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="16:19" x14ac:dyDescent="0.25">
-      <c r="P3" s="41" t="s">
+      <c r="P3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
     </row>
     <row r="4" spans="16:19" x14ac:dyDescent="0.25">
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
     </row>
     <row r="5" spans="16:19" x14ac:dyDescent="0.25">
-      <c r="P5" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="14" t="s">
+      <c r="P5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="14" t="s">
+      <c r="R5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="14" t="s">
+      <c r="S5" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1401,12 +1651,40 @@
         <v>49</v>
       </c>
     </row>
+    <row r="24" spans="16:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="P24" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q24" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="R24" s="32">
+        <v>360000</v>
+      </c>
+      <c r="S24" s="31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="16:21" x14ac:dyDescent="0.25">
+      <c r="P25" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q25" s="30">
+        <v>1</v>
+      </c>
+      <c r="R25" s="32">
+        <v>170000</v>
+      </c>
+      <c r="S25" s="31" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="31" spans="16:21" x14ac:dyDescent="0.25">
-      <c r="T31" s="31">
+      <c r="T31" s="24">
         <f>SUM(R6:R26)</f>
-        <v>2020000</v>
-      </c>
-      <c r="U31" s="13" t="s">
+        <v>2550000</v>
+      </c>
+      <c r="U31" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1422,55 +1700,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8BC094-5536-4558-8EA1-C96E0F45453E}">
   <dimension ref="J2:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
     </row>
     <row r="3" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
     </row>
     <row r="4" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="16" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J5" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="30">
+        <v>1</v>
+      </c>
+      <c r="L5" s="32">
+        <v>1800000</v>
+      </c>
+      <c r="M5" s="33">
+        <v>1800000</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J6" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="30">
+        <v>1</v>
+      </c>
+      <c r="L6" s="32">
+        <v>5150000</v>
+      </c>
+      <c r="M6" s="33">
+        <v>5150000</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O19" s="2">
         <f>SUM(M5:M10)</f>
-        <v>0</v>
-      </c>
-      <c r="P19" s="13" t="s">
+        <v>6950000</v>
+      </c>
+      <c r="P19" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1479,427 +1793,698 @@
     <mergeCell ref="J2:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FE7529-3FB2-4206-98A9-C20BF02B3565}">
-  <dimension ref="H3:N31"/>
+  <dimension ref="H2:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="39" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H3" s="42" t="s">
+    <row r="2" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="M2" s="24">
+        <f>SUM(K6:K41)</f>
+        <v>28796480</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-    </row>
-    <row r="4" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-    </row>
-    <row r="5" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H5" s="14" t="s">
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+    </row>
+    <row r="4" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+    </row>
+    <row r="5" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H5" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H6" s="18" t="s">
+    <row r="6" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H6" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="18">
-        <v>1</v>
-      </c>
-      <c r="J6" s="19">
+      <c r="I6" s="53">
+        <v>1</v>
+      </c>
+      <c r="J6" s="18">
         <v>230000</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="18">
         <f>(I6*J6)</f>
         <v>230000</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H7" s="18" t="s">
+    <row r="7" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H7" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="I7" s="18">
-        <v>1</v>
-      </c>
-      <c r="J7" s="19">
+      <c r="I7" s="53">
+        <v>1</v>
+      </c>
+      <c r="J7" s="18">
         <v>1360000</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="18">
         <f t="shared" ref="K7:K22" si="0">(I7*J7)</f>
         <v>1360000</v>
       </c>
-      <c r="L7" s="18" t="s">
+      <c r="L7" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H8" s="20" t="s">
+    <row r="8" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H8" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="53">
         <v>2</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="18">
         <v>65000</v>
       </c>
-      <c r="K8" s="21">
+      <c r="K8" s="18">
         <f t="shared" si="0"/>
         <v>130000</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H9" s="22" t="s">
+    <row r="9" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H9" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="22">
-        <v>1</v>
-      </c>
-      <c r="J9" s="23">
+      <c r="I9" s="53">
+        <v>1</v>
+      </c>
+      <c r="J9" s="18">
         <v>1050000</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="18">
         <f t="shared" si="0"/>
         <v>1050000</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H10" s="4" t="s">
+    <row r="10" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H10" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="4">
-        <v>1</v>
-      </c>
-      <c r="J10" s="5">
+      <c r="I10" s="53">
+        <v>1</v>
+      </c>
+      <c r="J10" s="18">
         <v>450000</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="18">
         <f t="shared" si="0"/>
         <v>450000</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H11" s="18" t="s">
+    <row r="11" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H11" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="53">
         <v>2</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="18">
         <v>30000</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="18">
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H12" s="22" t="s">
+    <row r="12" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H12" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="22">
-        <v>1</v>
-      </c>
-      <c r="J12" s="23">
+      <c r="I12" s="53">
+        <v>1</v>
+      </c>
+      <c r="J12" s="18">
         <v>190000</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="18">
         <f t="shared" si="0"/>
         <v>190000</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="L12" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H13" s="18" t="s">
+    <row r="13" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H13" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="18">
-        <v>1</v>
-      </c>
-      <c r="J13" s="19">
+      <c r="I13" s="53">
+        <v>1</v>
+      </c>
+      <c r="J13" s="18">
         <v>150000</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="18">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="L13" s="18" t="s">
+      <c r="L13" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H14" s="18" t="s">
+    <row r="14" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H14" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="I14" s="18">
-        <v>1</v>
-      </c>
-      <c r="J14" s="19">
+      <c r="I14" s="53">
+        <v>1</v>
+      </c>
+      <c r="J14" s="18">
         <v>115000</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="18">
         <f t="shared" si="0"/>
         <v>115000</v>
       </c>
-      <c r="L14" s="18" t="s">
+      <c r="L14" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H15" s="18" t="s">
+    <row r="15" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H15" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="18">
-        <v>1</v>
-      </c>
-      <c r="J15" s="19">
+      <c r="I15" s="53">
+        <v>1</v>
+      </c>
+      <c r="J15" s="18">
         <v>276000</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="18">
         <f t="shared" si="0"/>
         <v>276000</v>
       </c>
-      <c r="L15" s="18" t="s">
+      <c r="L15" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H16" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="I16" s="18">
-        <v>1</v>
-      </c>
-      <c r="J16" s="19">
+    <row r="16" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H16" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="53">
+        <v>1</v>
+      </c>
+      <c r="J16" s="18">
         <v>400000</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="18">
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
-      <c r="L16" s="18" t="s">
+      <c r="L16" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H17" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="18">
-        <v>1</v>
-      </c>
-      <c r="J17" s="19">
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H17" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" s="53">
+        <v>1</v>
+      </c>
+      <c r="J17" s="18">
         <v>120000</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="18">
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
-      <c r="L17" s="18" t="s">
+      <c r="L17" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H18" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="20">
-        <v>1</v>
-      </c>
-      <c r="J18" s="20">
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H18" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="53">
+        <v>1</v>
+      </c>
+      <c r="J18" s="18">
         <v>2372000</v>
       </c>
-      <c r="K18" s="21">
+      <c r="K18" s="18">
         <f t="shared" si="0"/>
         <v>2372000</v>
       </c>
-      <c r="L18" s="20" t="s">
+      <c r="L18" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H19" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I19" s="4">
-        <v>1</v>
-      </c>
-      <c r="J19" s="5">
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H19" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" s="53">
+        <v>1</v>
+      </c>
+      <c r="J19" s="18">
         <v>55000</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="18">
         <f t="shared" si="0"/>
         <v>55000</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H20" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I20" s="20">
-        <v>1</v>
-      </c>
-      <c r="J20" s="21">
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H20" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="53">
+        <v>1</v>
+      </c>
+      <c r="J20" s="18">
         <v>6536500</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K20" s="18">
         <f t="shared" si="0"/>
         <v>6536500</v>
       </c>
-      <c r="L20" s="20" t="s">
+      <c r="L20" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H21" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="22">
-        <v>1</v>
-      </c>
-      <c r="J21" s="23">
+    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H21" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" s="53">
+        <v>1</v>
+      </c>
+      <c r="J21" s="18">
         <v>3121980</v>
       </c>
-      <c r="K21" s="23">
+      <c r="K21" s="18">
         <f t="shared" si="0"/>
         <v>3121980</v>
       </c>
-      <c r="L21" s="22" t="s">
+      <c r="L21" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H22" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="I22" s="22">
-        <v>1</v>
-      </c>
-      <c r="J22" s="23">
+    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H22" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="53">
+        <v>1</v>
+      </c>
+      <c r="J22" s="18">
         <v>1980000</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="18">
         <f t="shared" si="0"/>
         <v>1980000</v>
       </c>
-      <c r="L22" s="22" t="s">
+      <c r="L22" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H23" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I23" s="4">
-        <v>1</v>
-      </c>
-      <c r="J23" s="5">
+    <row r="23" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H23" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23" s="53">
+        <v>1</v>
+      </c>
+      <c r="J23" s="18">
         <v>230000</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="18">
         <f>J23*I23</f>
         <v>230000</v>
       </c>
-      <c r="L23" s="22" t="s">
+      <c r="L23" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H24" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="I24" s="18">
+    <row r="24" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H24" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I24" s="53">
         <v>70</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="18">
         <v>9000</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24" s="18">
         <f t="shared" ref="K24:K25" si="1">J24*I24</f>
         <v>630000</v>
       </c>
-      <c r="L24" s="22" t="s">
+      <c r="L24" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H25" s="4" t="s">
+    <row r="25" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H25" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I25" s="53">
+        <v>70</v>
+      </c>
+      <c r="J25" s="18">
+        <v>10800</v>
+      </c>
+      <c r="K25" s="18">
+        <f t="shared" si="1"/>
+        <v>756000</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H26" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="I25" s="4">
-        <v>70</v>
-      </c>
-      <c r="J25" s="4">
-        <v>10500</v>
-      </c>
-      <c r="K25" s="25">
-        <f t="shared" si="1"/>
-        <v>735000</v>
-      </c>
-      <c r="L25" s="22" t="s">
+      <c r="I26" s="53">
+        <v>1</v>
+      </c>
+      <c r="J26" s="18">
+        <v>120000</v>
+      </c>
+      <c r="K26" s="18"/>
+      <c r="L26" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="M31" s="31">
-        <f>SUM(K6:K27)</f>
-        <v>20191480</v>
-      </c>
-      <c r="N31" s="13" t="s">
-        <v>4</v>
+    <row r="27" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H27" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="54">
+        <v>3</v>
+      </c>
+      <c r="J27" s="49">
+        <v>110000</v>
+      </c>
+      <c r="K27" s="50">
+        <v>330000</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="8:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="H28" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="I28" s="54">
+        <v>1</v>
+      </c>
+      <c r="J28" s="49">
+        <v>2125000</v>
+      </c>
+      <c r="K28" s="50">
+        <v>2125000</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H29" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="54">
+        <v>1</v>
+      </c>
+      <c r="J29" s="49">
+        <v>577000</v>
+      </c>
+      <c r="K29" s="50">
+        <v>577000</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H30" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="I30" s="54">
+        <v>10</v>
+      </c>
+      <c r="J30" s="49">
+        <v>11500</v>
+      </c>
+      <c r="K30" s="50">
+        <v>115000</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H31" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="I31" s="54">
+        <v>1</v>
+      </c>
+      <c r="J31" s="49">
+        <v>180000</v>
+      </c>
+      <c r="K31" s="50">
+        <v>180000</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H32" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="I32" s="54">
+        <v>1</v>
+      </c>
+      <c r="J32" s="49">
+        <v>260000</v>
+      </c>
+      <c r="K32" s="50">
+        <v>260000</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="8:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="H33" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="I33" s="54">
+        <v>1</v>
+      </c>
+      <c r="J33" s="49">
+        <v>122000</v>
+      </c>
+      <c r="K33" s="50">
+        <v>122000</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H34" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="I34" s="54">
+        <v>1</v>
+      </c>
+      <c r="J34" s="49">
+        <v>120000</v>
+      </c>
+      <c r="K34" s="50">
+        <v>120000</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="8:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="H35" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="I35" s="54">
+        <v>1</v>
+      </c>
+      <c r="J35" s="49">
+        <v>928000</v>
+      </c>
+      <c r="K35" s="50">
+        <v>928000</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="8:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="H36" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="I36" s="54">
+        <v>1</v>
+      </c>
+      <c r="J36" s="49">
+        <v>222000</v>
+      </c>
+      <c r="K36" s="50">
+        <v>222000</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H37" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="I37" s="54">
+        <v>1</v>
+      </c>
+      <c r="J37" s="49">
+        <v>200000</v>
+      </c>
+      <c r="K37" s="50">
+        <v>200000</v>
+      </c>
+      <c r="L37" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H38" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="I38" s="54">
+        <v>1</v>
+      </c>
+      <c r="J38" s="49">
+        <v>1750000</v>
+      </c>
+      <c r="K38" s="50">
+        <v>1750000</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="8:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="H39" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="I39" s="54">
+        <v>1</v>
+      </c>
+      <c r="J39" s="49">
+        <v>500000</v>
+      </c>
+      <c r="K39" s="50">
+        <v>500000</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H40" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="I40" s="54">
+        <v>1</v>
+      </c>
+      <c r="J40" s="49">
+        <v>1000000</v>
+      </c>
+      <c r="K40" s="50">
+        <v>1000000</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H41" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" s="54">
+        <v>1</v>
+      </c>
+      <c r="J41" s="49">
+        <v>155000</v>
+      </c>
+      <c r="K41" s="50">
+        <v>155000</v>
+      </c>
+      <c r="L41" s="17" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1907,6 +2492,7 @@
     <mergeCell ref="H3:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1914,92 +2500,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF898539-51C6-4967-9BBB-301946D3AEB1}">
   <dimension ref="I4:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I4" s="41" t="s">
+    <row r="4" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I4" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-    </row>
-    <row r="5" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-    </row>
-    <row r="6" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I6" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="26" t="s">
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+    </row>
+    <row r="5" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+    </row>
+    <row r="6" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="35" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J7" s="5">
         <v>2000000</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="9:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="I8" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="32">
+        <v>250000</v>
+      </c>
+      <c r="K8" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="31"/>
+    </row>
+    <row r="9" spans="9:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="I9" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="32">
+        <v>1000000</v>
+      </c>
+      <c r="K9" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" s="31"/>
+    </row>
+    <row r="10" spans="9:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="32">
+        <v>1880000</v>
+      </c>
+      <c r="K10" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="31"/>
+    </row>
+    <row r="11" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I11" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="32">
+        <v>1200000</v>
+      </c>
+      <c r="K11" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="31"/>
+    </row>
+    <row r="12" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="36"/>
+    </row>
+    <row r="13" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I13" s="4"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="36"/>
+    </row>
+    <row r="14" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="4"/>
+      <c r="K14" s="36"/>
     </row>
     <row r="20" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L20" s="2">
         <f>SUM(J7:J13)</f>
-        <v>2000000</v>
-      </c>
-      <c r="M20" s="13" t="s">
+        <v>6330000</v>
+      </c>
+      <c r="M20" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2026,39 +2640,39 @@
   </cols>
   <sheetData>
     <row r="5" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
+      <c r="H5" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
     </row>
     <row r="6" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
     </row>
     <row r="7" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H7" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J7" s="30" t="s">
+      <c r="H7" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J8" s="5">
         <v>3600000</v>
@@ -2150,7 +2764,7 @@
         <f>SUM(J8:J19)</f>
         <v>3600000</v>
       </c>
-      <c r="M26" s="13" t="s">
+      <c r="M26" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2160,4 +2774,105 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48045ABA-9A5B-4D55-856F-C5AF2ED54280}">
+  <dimension ref="K3:P11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" style="39" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="11:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="O3" s="46">
+        <f>SUM(M6:M13)</f>
+        <v>37174000</v>
+      </c>
+      <c r="P3" s="47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="11:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+    </row>
+    <row r="5" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K5" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="M5" s="43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="44">
+        <v>44412</v>
+      </c>
+      <c r="M6" s="5">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="7" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="M7" s="5">
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="8" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L8" s="45"/>
+      <c r="M8" s="68">
+        <v>7174000</v>
+      </c>
+    </row>
+    <row r="9" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K9" s="4"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K10" s="4"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K11" s="4"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K3:M4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>